<commit_message>
start of step 1, roster dataset
</commit_message>
<xml_diff>
--- a/input/dataset/data.xlsx
+++ b/input/dataset/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNAEdu/Analysis/MSNAEducation/input/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="247" documentId="8_{F8FA1124-47E3-41F7-BA8D-0049A8410AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5EE1C02-B331-4513-8FCB-A236A7C7A6DD}"/>
+  <xr:revisionPtr revIDLastSave="258" documentId="8_{F8FA1124-47E3-41F7-BA8D-0049A8410AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E3F38E6-D927-4951-85A4-9A72E399F57B}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11265" xr2:uid="{6675326B-8B2D-4F8E-8948-650575623738}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11265" activeTab="1" xr2:uid="{6675326B-8B2D-4F8E-8948-650575623738}"/>
   </bookViews>
   <sheets>
     <sheet name="HH loop" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="69">
   <si>
     <t>uuid</t>
   </si>
@@ -222,15 +222,6 @@
     <t>primary, year2</t>
   </si>
   <si>
-    <t>kindergarden</t>
-  </si>
-  <si>
-    <t>upper secondary, year1</t>
-  </si>
-  <si>
-    <t>intermediate, year1</t>
-  </si>
-  <si>
     <t>cash</t>
   </si>
   <si>
@@ -238,6 +229,21 @@
   </si>
   <si>
     <t>pippo</t>
+  </si>
+  <si>
+    <t>upper secondary, year12</t>
+  </si>
+  <si>
+    <t>lower secondary, year9</t>
+  </si>
+  <si>
+    <t>primary, year7</t>
+  </si>
+  <si>
+    <t>primary, year5</t>
+  </si>
+  <si>
+    <t>primary, year3</t>
   </si>
 </sst>
 </file>
@@ -665,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89BADB42-A13D-41D4-92FA-299C3FB67C7A}">
   <dimension ref="A1:K10438"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -787,7 +793,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -1393,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D8463A-BC38-4B3C-A2FA-F7194594359A}">
   <dimension ref="A1:O54049"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1461,7 +1467,7 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -1494,7 +1500,7 @@
         <v>12</v>
       </c>
       <c r="O2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.75">
@@ -1608,7 +1614,7 @@
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
         <v>12</v>
@@ -1752,7 +1758,7 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H8" t="s">
         <v>12</v>
@@ -1776,7 +1782,7 @@
         <v>57</v>
       </c>
       <c r="O8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.75">
@@ -1796,7 +1802,7 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G9" t="s">
         <v>12</v>
@@ -1890,7 +1896,7 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G11" t="s">
         <v>12</v>
@@ -1937,7 +1943,7 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
@@ -1964,7 +1970,7 @@
         <v>12</v>
       </c>
       <c r="O12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.75">
@@ -2078,7 +2084,7 @@
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="G15" t="s">
         <v>12</v>
@@ -2172,7 +2178,7 @@
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G17" t="s">
         <v>12</v>
@@ -2199,7 +2205,7 @@
         <v>12</v>
       </c>
       <c r="O17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
end of the week, adding simple numerator and denominator. Missing level and grade reading function
</commit_message>
<xml_diff>
--- a/input/dataset/data.xlsx
+++ b/input/dataset/data.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="258" documentId="8_{F8FA1124-47E3-41F7-BA8D-0049A8410AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E3F38E6-D927-4951-85A4-9A72E399F57B}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11265" activeTab="1" xr2:uid="{6675326B-8B2D-4F8E-8948-650575623738}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11265" xr2:uid="{6675326B-8B2D-4F8E-8948-650575623738}"/>
   </bookViews>
   <sheets>
     <sheet name="HH loop" sheetId="1" r:id="rId1"/>
@@ -671,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89BADB42-A13D-41D4-92FA-299C3FB67C7A}">
   <dimension ref="A1:K10438"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1399,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D8463A-BC38-4B3C-A2FA-F7194594359A}">
   <dimension ref="A1:O54049"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>

</xml_diff>

<commit_message>
adding unesco file, reading grades from the file, adding indicators dynimically
</commit_message>
<xml_diff>
--- a/input/dataset/data.xlsx
+++ b/input/dataset/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNAEdu/Analysis/MSNAEducation/input/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="260" documentId="8_{F8FA1124-47E3-41F7-BA8D-0049A8410AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D7E33AB-EB38-4CE0-974A-156002DBF010}"/>
+  <xr:revisionPtr revIDLastSave="271" documentId="8_{F8FA1124-47E3-41F7-BA8D-0049A8410AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{423DEBA3-B1EC-4C7E-AB8E-7EE2ADE676DE}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11265" activeTab="1" xr2:uid="{6675326B-8B2D-4F8E-8948-650575623738}"/>
   </bookViews>
@@ -216,12 +216,6 @@
     <t>madrasa</t>
   </si>
   <si>
-    <t>primary, year1</t>
-  </si>
-  <si>
-    <t>primary, year2</t>
-  </si>
-  <si>
     <t>cash</t>
   </si>
   <si>
@@ -231,19 +225,25 @@
     <t>pippo</t>
   </si>
   <si>
-    <t>lower secondary, year9</t>
+    <t>Primary_Grade_1</t>
   </si>
   <si>
-    <t>primary, year7</t>
+    <t>Primary_Grade_2</t>
   </si>
   <si>
-    <t>primary, year5</t>
+    <t>Primary_Grade_5</t>
   </si>
   <si>
-    <t>primary, year3</t>
+    <t>Primary_Grade_3</t>
   </si>
   <si>
-    <t>secondaire deuxième cycle, year12</t>
+    <t>Primary_Grade_7</t>
+  </si>
+  <si>
+    <t>Lower_Secondary_Grade_9</t>
+  </si>
+  <si>
+    <t>Upper_Secondary_Grade_10</t>
   </si>
 </sst>
 </file>
@@ -270,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +293,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -323,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -335,6 +341,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,7 +800,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -1400,13 +1407,13 @@
   <dimension ref="A1:O54049"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="4" max="4" width="11.90625" customWidth="1"/>
-    <col min="6" max="6" width="27.6796875" customWidth="1"/>
+    <col min="6" max="6" width="40.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="60" x14ac:dyDescent="0.75">
@@ -1473,7 +1480,7 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1500,7 +1507,7 @@
         <v>12</v>
       </c>
       <c r="O2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.75">
@@ -1550,50 +1557,50 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
+    <row r="4" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="F4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="M4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="M4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1614,7 +1621,7 @@
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
         <v>12</v>
@@ -1758,7 +1765,7 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H8" t="s">
         <v>12</v>
@@ -1782,7 +1789,7 @@
         <v>57</v>
       </c>
       <c r="O8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.75">
@@ -1802,7 +1809,7 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G9" t="s">
         <v>12</v>
@@ -1896,7 +1903,7 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G11" t="s">
         <v>12</v>
@@ -1943,7 +1950,7 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
@@ -1970,7 +1977,7 @@
         <v>12</v>
       </c>
       <c r="O12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.75">
@@ -2084,7 +2091,7 @@
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G15" t="s">
         <v>12</v>
@@ -2178,7 +2185,7 @@
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G17" t="s">
         <v>12</v>
@@ -2205,7 +2212,7 @@
         <v>12</v>
       </c>
       <c r="O17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
to be changed again
</commit_message>
<xml_diff>
--- a/input/dataset/data.xlsx
+++ b/input/dataset/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNAEdu/Analysis/MSNAEducation/input/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="271" documentId="8_{F8FA1124-47E3-41F7-BA8D-0049A8410AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{423DEBA3-B1EC-4C7E-AB8E-7EE2ADE676DE}"/>
+  <xr:revisionPtr revIDLastSave="274" documentId="8_{F8FA1124-47E3-41F7-BA8D-0049A8410AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AEC9D6D-7602-4FC3-84D2-D04827FA7BBB}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11265" activeTab="1" xr2:uid="{6675326B-8B2D-4F8E-8948-650575623738}"/>
   </bookViews>
@@ -1407,7 +1407,7 @@
   <dimension ref="A1:O54049"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1803,7 +1803,7 @@
         <v>18</v>
       </c>
       <c r="D9">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
all the indicators are added!!!
</commit_message>
<xml_diff>
--- a/input/dataset/data.xlsx
+++ b/input/dataset/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNAEdu/Analysis/MSNAEducation/input/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="274" documentId="8_{F8FA1124-47E3-41F7-BA8D-0049A8410AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AEC9D6D-7602-4FC3-84D2-D04827FA7BBB}"/>
+  <xr:revisionPtr revIDLastSave="282" documentId="8_{F8FA1124-47E3-41F7-BA8D-0049A8410AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E37B46B-8C18-42BB-84C1-E1BD5BD316B3}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11265" activeTab="1" xr2:uid="{6675326B-8B2D-4F8E-8948-650575623738}"/>
   </bookViews>
@@ -225,25 +225,25 @@
     <t>pippo</t>
   </si>
   <si>
-    <t>Primary_Grade_1</t>
+    <t>primary_grade_1</t>
   </si>
   <si>
-    <t>Primary_Grade_2</t>
+    <t>primary_grade_2</t>
   </si>
   <si>
-    <t>Primary_Grade_5</t>
+    <t>primary_grade_5</t>
   </si>
   <si>
-    <t>Primary_Grade_3</t>
+    <t>primary_grade_3</t>
   </si>
   <si>
-    <t>Primary_Grade_7</t>
+    <t>primary_grade_7</t>
   </si>
   <si>
-    <t>Lower_Secondary_Grade_9</t>
+    <t>lower_secondary_grade_9</t>
   </si>
   <si>
-    <t>Upper_Secondary_Grade_10</t>
+    <t>upper_secondary_grade_10</t>
   </si>
 </sst>
 </file>
@@ -1407,7 +1407,7 @@
   <dimension ref="A1:O54049"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1568,7 +1568,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>25</v>
@@ -1803,7 +1803,7 @@
         <v>18</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
going for resource (excel) based input. WGSS done
</commit_message>
<xml_diff>
--- a/input/dataset/data.xlsx
+++ b/input/dataset/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNAEdu/Analysis/MSNAEducation/input/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="293" documentId="8_{F8FA1124-47E3-41F7-BA8D-0049A8410AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7592643-7587-4107-8318-B7627CE19A7A}"/>
+  <xr:revisionPtr revIDLastSave="304" documentId="8_{F8FA1124-47E3-41F7-BA8D-0049A8410AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{724387E6-D989-4B57-9CC6-01F5CAEDBF22}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11265" activeTab="1" xr2:uid="{6675326B-8B2D-4F8E-8948-650575623738}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11265" activeTab="2" xr2:uid="{6675326B-8B2D-4F8E-8948-650575623738}"/>
   </bookViews>
   <sheets>
     <sheet name="HH loop" sheetId="1" r:id="rId1"/>
@@ -259,13 +259,7 @@
     <t>difficulty_self_care</t>
   </si>
   <si>
-    <t>difficulty_communicating</t>
-  </si>
-  <si>
     <t>a_lot_of_difficulty</t>
-  </si>
-  <si>
-    <t>no_difficulty</t>
   </si>
   <si>
     <t>cannot_do_at_all</t>
@@ -277,7 +271,13 @@
     <t>some_difficulty</t>
   </si>
   <si>
-    <t>primary_grade_7</t>
+    <t>primary_grade_6</t>
+  </si>
+  <si>
+    <t>difficulty_communicating</t>
+  </si>
+  <si>
+    <t>none_difficulty</t>
   </si>
 </sst>
 </file>
@@ -1440,13 +1440,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D8463A-BC38-4B3C-A2FA-F7194594359A}">
   <dimension ref="A1:O54049"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="4" max="4" width="11.90625" customWidth="1"/>
+    <col min="4" max="4" width="11.86328125" customWidth="1"/>
     <col min="6" max="6" width="40.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2219,7 +2219,7 @@
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G17" t="s">
         <v>12</v>
@@ -8240,13 +8240,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E5E3D4-B3C4-4861-8FC5-05A8FCCE6E1C}">
   <dimension ref="A1:J54049"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="4" max="4" width="11.90625" customWidth="1"/>
+    <col min="4" max="4" width="11.86328125" customWidth="1"/>
+    <col min="5" max="11" width="17.2265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.75">
@@ -8278,7 +8279,7 @@
         <v>72</v>
       </c>
       <c r="J1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.75">
@@ -8295,22 +8296,22 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.75">
@@ -8327,22 +8328,22 @@
         <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.75">
@@ -8359,22 +8360,22 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" t="s">
         <v>76</v>
-      </c>
-      <c r="F4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I4" t="s">
-        <v>75</v>
-      </c>
-      <c r="J4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.75">
@@ -8391,22 +8392,22 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" t="s">
         <v>76</v>
       </c>
-      <c r="F5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5" t="s">
-        <v>78</v>
-      </c>
       <c r="J5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.75">
@@ -8423,22 +8424,22 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.75">
@@ -8455,22 +8456,22 @@
         <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.75">
@@ -8487,22 +8488,22 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" t="s">
         <v>75</v>
-      </c>
-      <c r="H8" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" t="s">
-        <v>75</v>
-      </c>
-      <c r="J8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.75">
@@ -8519,22 +8520,22 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" t="s">
         <v>76</v>
       </c>
-      <c r="F9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="J9" t="s">
         <v>75</v>
-      </c>
-      <c r="H9" t="s">
-        <v>75</v>
-      </c>
-      <c r="I9" t="s">
-        <v>78</v>
-      </c>
-      <c r="J9" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.75">
@@ -8551,22 +8552,22 @@
         <v>17</v>
       </c>
       <c r="E10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" t="s">
         <v>76</v>
       </c>
-      <c r="F10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H10" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" t="s">
-        <v>78</v>
-      </c>
       <c r="J10" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.75">
@@ -8583,22 +8584,22 @@
         <v>15</v>
       </c>
       <c r="E11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" t="s">
         <v>76</v>
       </c>
-      <c r="F11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" t="s">
-        <v>78</v>
-      </c>
       <c r="J11" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.75">
@@ -8615,22 +8616,22 @@
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" t="s">
         <v>75</v>
-      </c>
-      <c r="H12" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" t="s">
-        <v>75</v>
-      </c>
-      <c r="J12" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.75">
@@ -8647,22 +8648,22 @@
         <v>4</v>
       </c>
       <c r="E13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" t="s">
         <v>76</v>
       </c>
-      <c r="F13" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" t="s">
-        <v>78</v>
-      </c>
       <c r="J13" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.75">
@@ -8679,22 +8680,22 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" t="s">
         <v>76</v>
       </c>
-      <c r="F14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="J14" t="s">
         <v>75</v>
-      </c>
-      <c r="H14" t="s">
-        <v>77</v>
-      </c>
-      <c r="I14" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.75">
@@ -8711,22 +8712,22 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H15" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I15" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.75">
@@ -8743,22 +8744,22 @@
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G16" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I16" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J16" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.75">
@@ -8775,22 +8776,22 @@
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H17" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I17" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J17" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
working on creating the package function for HUMIND
</commit_message>
<xml_diff>
--- a/input/dataset/data.xlsx
+++ b/input/dataset/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNAEdu/Analysis/MSNAEducation/input/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="304" documentId="8_{F8FA1124-47E3-41F7-BA8D-0049A8410AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{724387E6-D989-4B57-9CC6-01F5CAEDBF22}"/>
+  <xr:revisionPtr revIDLastSave="318" documentId="8_{F8FA1124-47E3-41F7-BA8D-0049A8410AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D77BB2AA-EE4C-47B3-8683-5C7CEE0297FF}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11265" activeTab="2" xr2:uid="{6675326B-8B2D-4F8E-8948-650575623738}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11265" activeTab="1" xr2:uid="{6675326B-8B2D-4F8E-8948-650575623738}"/>
   </bookViews>
   <sheets>
     <sheet name="HH loop" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="80">
   <si>
     <t>uuid</t>
   </si>
@@ -1440,12 +1440,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D8463A-BC38-4B3C-A2FA-F7194594359A}">
   <dimension ref="A1:O54049"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="11.86328125" customWidth="1"/>
     <col min="6" max="6" width="40.54296875" customWidth="1"/>
   </cols>
@@ -2071,14 +2072,14 @@
       <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
-        <v>12</v>
+      <c r="D14">
+        <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G14" t="s">
         <v>12</v>
@@ -2087,16 +2088,16 @@
         <v>12</v>
       </c>
       <c r="I14" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="J14" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="K14" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="L14" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="M14" t="s">
         <v>12</v>
@@ -2105,7 +2106,7 @@
         <v>12</v>
       </c>
       <c r="O14" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.75">
@@ -2249,24 +2250,2543 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B66" s="1"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B67" s="1"/>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18" t="s">
+        <v>12</v>
+      </c>
+      <c r="O18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" t="s">
+        <v>12</v>
+      </c>
+      <c r="M19" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19" t="s">
+        <v>12</v>
+      </c>
+      <c r="O19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="5">
+        <v>14</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" t="s">
+        <v>25</v>
+      </c>
+      <c r="L21" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" t="s">
+        <v>12</v>
+      </c>
+      <c r="N21" t="s">
+        <v>12</v>
+      </c>
+      <c r="O21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" t="s">
+        <v>12</v>
+      </c>
+      <c r="L22" t="s">
+        <v>12</v>
+      </c>
+      <c r="M22" t="s">
+        <v>12</v>
+      </c>
+      <c r="N22" t="s">
+        <v>12</v>
+      </c>
+      <c r="O22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" t="s">
+        <v>12</v>
+      </c>
+      <c r="M23" t="s">
+        <v>12</v>
+      </c>
+      <c r="N23" t="s">
+        <v>12</v>
+      </c>
+      <c r="O23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" t="s">
+        <v>12</v>
+      </c>
+      <c r="L24" t="s">
+        <v>12</v>
+      </c>
+      <c r="M24" t="s">
+        <v>25</v>
+      </c>
+      <c r="N24" t="s">
+        <v>57</v>
+      </c>
+      <c r="O24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25">
+        <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" t="s">
+        <v>12</v>
+      </c>
+      <c r="M25" t="s">
+        <v>12</v>
+      </c>
+      <c r="N25" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" t="s">
+        <v>12</v>
+      </c>
+      <c r="J26" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" t="s">
+        <v>12</v>
+      </c>
+      <c r="L26" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" t="s">
+        <v>12</v>
+      </c>
+      <c r="N26" t="s">
+        <v>58</v>
+      </c>
+      <c r="O26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" t="s">
+        <v>27</v>
+      </c>
+      <c r="K27" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M27" t="s">
+        <v>25</v>
+      </c>
+      <c r="N27" t="s">
+        <v>12</v>
+      </c>
+      <c r="O27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N28" t="s">
+        <v>12</v>
+      </c>
+      <c r="O28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" t="s">
+        <v>12</v>
+      </c>
+      <c r="M29" t="s">
+        <v>12</v>
+      </c>
+      <c r="N29" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30" t="s">
+        <v>25</v>
+      </c>
+      <c r="K30" t="s">
+        <v>27</v>
+      </c>
+      <c r="L30" t="s">
+        <v>27</v>
+      </c>
+      <c r="M30" t="s">
+        <v>12</v>
+      </c>
+      <c r="N30" t="s">
+        <v>12</v>
+      </c>
+      <c r="O30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" t="s">
+        <v>27</v>
+      </c>
+      <c r="J31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K31" t="s">
+        <v>25</v>
+      </c>
+      <c r="L31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" t="s">
+        <v>12</v>
+      </c>
+      <c r="N31" t="s">
+        <v>12</v>
+      </c>
+      <c r="O31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" t="s">
+        <v>12</v>
+      </c>
+      <c r="K32" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" t="s">
+        <v>12</v>
+      </c>
+      <c r="M32" t="s">
+        <v>27</v>
+      </c>
+      <c r="N32" t="s">
+        <v>12</v>
+      </c>
+      <c r="O32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>77</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s">
+        <v>12</v>
+      </c>
+      <c r="I33" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K33" t="s">
+        <v>25</v>
+      </c>
+      <c r="L33" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" t="s">
+        <v>12</v>
+      </c>
+      <c r="N33" t="s">
+        <v>12</v>
+      </c>
+      <c r="O33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s">
+        <v>12</v>
+      </c>
+      <c r="I34" t="s">
+        <v>25</v>
+      </c>
+      <c r="J34" t="s">
+        <v>25</v>
+      </c>
+      <c r="K34" t="s">
+        <v>27</v>
+      </c>
+      <c r="L34" t="s">
+        <v>27</v>
+      </c>
+      <c r="M34" t="s">
+        <v>12</v>
+      </c>
+      <c r="N34" t="s">
+        <v>12</v>
+      </c>
+      <c r="O34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35">
+        <v>23</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" t="s">
+        <v>12</v>
+      </c>
+      <c r="M35" t="s">
+        <v>12</v>
+      </c>
+      <c r="N35" t="s">
+        <v>12</v>
+      </c>
+      <c r="O35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="5">
+        <v>14</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" t="s">
+        <v>27</v>
+      </c>
+      <c r="J37" t="s">
+        <v>27</v>
+      </c>
+      <c r="K37" t="s">
+        <v>25</v>
+      </c>
+      <c r="L37" t="s">
+        <v>27</v>
+      </c>
+      <c r="M37" t="s">
+        <v>12</v>
+      </c>
+      <c r="N37" t="s">
+        <v>12</v>
+      </c>
+      <c r="O37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" t="s">
+        <v>12</v>
+      </c>
+      <c r="J38" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38" t="s">
+        <v>12</v>
+      </c>
+      <c r="L38" t="s">
+        <v>12</v>
+      </c>
+      <c r="M38" t="s">
+        <v>12</v>
+      </c>
+      <c r="N38" t="s">
+        <v>12</v>
+      </c>
+      <c r="O38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39">
+        <v>45</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" t="s">
+        <v>12</v>
+      </c>
+      <c r="J39" t="s">
+        <v>12</v>
+      </c>
+      <c r="K39" t="s">
+        <v>12</v>
+      </c>
+      <c r="L39" t="s">
+        <v>12</v>
+      </c>
+      <c r="M39" t="s">
+        <v>12</v>
+      </c>
+      <c r="N39" t="s">
+        <v>12</v>
+      </c>
+      <c r="O39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" t="s">
+        <v>60</v>
+      </c>
+      <c r="H40" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" t="s">
+        <v>12</v>
+      </c>
+      <c r="J40" t="s">
+        <v>12</v>
+      </c>
+      <c r="K40" t="s">
+        <v>12</v>
+      </c>
+      <c r="L40" t="s">
+        <v>12</v>
+      </c>
+      <c r="M40" t="s">
+        <v>25</v>
+      </c>
+      <c r="N40" t="s">
+        <v>57</v>
+      </c>
+      <c r="O40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41">
+        <v>19</v>
+      </c>
+      <c r="E41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" t="s">
+        <v>66</v>
+      </c>
+      <c r="G41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" t="s">
+        <v>12</v>
+      </c>
+      <c r="J41" t="s">
+        <v>12</v>
+      </c>
+      <c r="K41" t="s">
+        <v>12</v>
+      </c>
+      <c r="L41" t="s">
+        <v>12</v>
+      </c>
+      <c r="M41" t="s">
+        <v>12</v>
+      </c>
+      <c r="N41" t="s">
+        <v>12</v>
+      </c>
+      <c r="O41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42">
+        <v>17</v>
+      </c>
+      <c r="E42" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" t="s">
+        <v>33</v>
+      </c>
+      <c r="H42" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" t="s">
+        <v>12</v>
+      </c>
+      <c r="J42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L42" t="s">
+        <v>12</v>
+      </c>
+      <c r="M42" t="s">
+        <v>12</v>
+      </c>
+      <c r="N42" t="s">
+        <v>58</v>
+      </c>
+      <c r="O42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43">
+        <v>15</v>
+      </c>
+      <c r="E43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" t="s">
+        <v>67</v>
+      </c>
+      <c r="G43" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" t="s">
+        <v>27</v>
+      </c>
+      <c r="J43" t="s">
+        <v>27</v>
+      </c>
+      <c r="K43" t="s">
+        <v>25</v>
+      </c>
+      <c r="L43" t="s">
+        <v>56</v>
+      </c>
+      <c r="M43" t="s">
+        <v>25</v>
+      </c>
+      <c r="N43" t="s">
+        <v>12</v>
+      </c>
+      <c r="O43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44">
+        <v>13</v>
+      </c>
+      <c r="E44" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" t="s">
+        <v>25</v>
+      </c>
+      <c r="J44" t="s">
+        <v>25</v>
+      </c>
+      <c r="K44" t="s">
+        <v>25</v>
+      </c>
+      <c r="L44" t="s">
+        <v>25</v>
+      </c>
+      <c r="M44" t="s">
+        <v>12</v>
+      </c>
+      <c r="N44" t="s">
+        <v>12</v>
+      </c>
+      <c r="O44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" t="s">
+        <v>12</v>
+      </c>
+      <c r="J45" t="s">
+        <v>12</v>
+      </c>
+      <c r="K45" t="s">
+        <v>12</v>
+      </c>
+      <c r="L45" t="s">
+        <v>12</v>
+      </c>
+      <c r="M45" t="s">
+        <v>12</v>
+      </c>
+      <c r="N45" t="s">
+        <v>12</v>
+      </c>
+      <c r="O45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" t="s">
+        <v>62</v>
+      </c>
+      <c r="G46" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" t="s">
+        <v>25</v>
+      </c>
+      <c r="J46" t="s">
+        <v>25</v>
+      </c>
+      <c r="K46" t="s">
+        <v>27</v>
+      </c>
+      <c r="L46" t="s">
+        <v>27</v>
+      </c>
+      <c r="M46" t="s">
+        <v>12</v>
+      </c>
+      <c r="N46" t="s">
+        <v>12</v>
+      </c>
+      <c r="O46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" t="s">
+        <v>65</v>
+      </c>
+      <c r="G47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s">
+        <v>12</v>
+      </c>
+      <c r="I47" t="s">
+        <v>27</v>
+      </c>
+      <c r="J47" t="s">
+        <v>27</v>
+      </c>
+      <c r="K47" t="s">
+        <v>25</v>
+      </c>
+      <c r="L47" t="s">
+        <v>25</v>
+      </c>
+      <c r="M47" t="s">
+        <v>12</v>
+      </c>
+      <c r="N47" t="s">
+        <v>12</v>
+      </c>
+      <c r="O47" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48">
+        <v>15</v>
+      </c>
+      <c r="E48" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" t="s">
+        <v>40</v>
+      </c>
+      <c r="H48" t="s">
+        <v>12</v>
+      </c>
+      <c r="I48" t="s">
+        <v>12</v>
+      </c>
+      <c r="J48" t="s">
+        <v>12</v>
+      </c>
+      <c r="K48" t="s">
+        <v>12</v>
+      </c>
+      <c r="L48" t="s">
+        <v>12</v>
+      </c>
+      <c r="M48" t="s">
+        <v>27</v>
+      </c>
+      <c r="N48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O48" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49">
+        <v>12</v>
+      </c>
+      <c r="E49" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" t="s">
+        <v>77</v>
+      </c>
+      <c r="G49" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" t="s">
+        <v>12</v>
+      </c>
+      <c r="I49" t="s">
+        <v>25</v>
+      </c>
+      <c r="J49" t="s">
+        <v>25</v>
+      </c>
+      <c r="K49" t="s">
+        <v>25</v>
+      </c>
+      <c r="L49" t="s">
+        <v>27</v>
+      </c>
+      <c r="M49" t="s">
+        <v>12</v>
+      </c>
+      <c r="N49" t="s">
+        <v>12</v>
+      </c>
+      <c r="O49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50">
+        <v>6</v>
+      </c>
+      <c r="E50" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" t="s">
+        <v>62</v>
+      </c>
+      <c r="G50" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" t="s">
+        <v>12</v>
+      </c>
+      <c r="I50" t="s">
+        <v>25</v>
+      </c>
+      <c r="J50" t="s">
+        <v>25</v>
+      </c>
+      <c r="K50" t="s">
+        <v>27</v>
+      </c>
+      <c r="L50" t="s">
+        <v>27</v>
+      </c>
+      <c r="M50" t="s">
+        <v>12</v>
+      </c>
+      <c r="N50" t="s">
+        <v>12</v>
+      </c>
+      <c r="O50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51">
+        <v>23</v>
+      </c>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" t="s">
+        <v>12</v>
+      </c>
+      <c r="I51" t="s">
+        <v>12</v>
+      </c>
+      <c r="J51" t="s">
+        <v>12</v>
+      </c>
+      <c r="K51" t="s">
+        <v>12</v>
+      </c>
+      <c r="L51" t="s">
+        <v>12</v>
+      </c>
+      <c r="M51" t="s">
+        <v>12</v>
+      </c>
+      <c r="N51" t="s">
+        <v>12</v>
+      </c>
+      <c r="O51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A52" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="5">
+        <v>14</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O52" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A53" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53">
+        <v>8</v>
+      </c>
+      <c r="E53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" t="s">
+        <v>63</v>
+      </c>
+      <c r="G53" t="s">
+        <v>12</v>
+      </c>
+      <c r="H53" t="s">
+        <v>12</v>
+      </c>
+      <c r="I53" t="s">
+        <v>27</v>
+      </c>
+      <c r="J53" t="s">
+        <v>27</v>
+      </c>
+      <c r="K53" t="s">
+        <v>25</v>
+      </c>
+      <c r="L53" t="s">
+        <v>27</v>
+      </c>
+      <c r="M53" t="s">
+        <v>12</v>
+      </c>
+      <c r="N53" t="s">
+        <v>12</v>
+      </c>
+      <c r="O53" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" t="s">
+        <v>12</v>
+      </c>
+      <c r="I54" t="s">
+        <v>12</v>
+      </c>
+      <c r="J54" t="s">
+        <v>12</v>
+      </c>
+      <c r="K54" t="s">
+        <v>12</v>
+      </c>
+      <c r="L54" t="s">
+        <v>12</v>
+      </c>
+      <c r="M54" t="s">
+        <v>12</v>
+      </c>
+      <c r="N54" t="s">
+        <v>12</v>
+      </c>
+      <c r="O54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55">
+        <v>45</v>
+      </c>
+      <c r="E55" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55" t="s">
+        <v>12</v>
+      </c>
+      <c r="I55" t="s">
+        <v>12</v>
+      </c>
+      <c r="J55" t="s">
+        <v>12</v>
+      </c>
+      <c r="K55" t="s">
+        <v>12</v>
+      </c>
+      <c r="L55" t="s">
+        <v>12</v>
+      </c>
+      <c r="M55" t="s">
+        <v>12</v>
+      </c>
+      <c r="N55" t="s">
+        <v>12</v>
+      </c>
+      <c r="O55" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56">
+        <v>9</v>
+      </c>
+      <c r="E56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" t="s">
+        <v>60</v>
+      </c>
+      <c r="H56" t="s">
+        <v>12</v>
+      </c>
+      <c r="I56" t="s">
+        <v>12</v>
+      </c>
+      <c r="J56" t="s">
+        <v>12</v>
+      </c>
+      <c r="K56" t="s">
+        <v>12</v>
+      </c>
+      <c r="L56" t="s">
+        <v>12</v>
+      </c>
+      <c r="M56" t="s">
+        <v>25</v>
+      </c>
+      <c r="N56" t="s">
+        <v>57</v>
+      </c>
+      <c r="O56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" t="s">
+        <v>31</v>
+      </c>
+      <c r="C57" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57">
+        <v>19</v>
+      </c>
+      <c r="E57" t="s">
+        <v>25</v>
+      </c>
+      <c r="F57" t="s">
+        <v>66</v>
+      </c>
+      <c r="G57" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" t="s">
+        <v>12</v>
+      </c>
+      <c r="I57" t="s">
+        <v>12</v>
+      </c>
+      <c r="J57" t="s">
+        <v>12</v>
+      </c>
+      <c r="K57" t="s">
+        <v>12</v>
+      </c>
+      <c r="L57" t="s">
+        <v>12</v>
+      </c>
+      <c r="M57" t="s">
+        <v>12</v>
+      </c>
+      <c r="N57" t="s">
+        <v>12</v>
+      </c>
+      <c r="O57" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58">
+        <v>17</v>
+      </c>
+      <c r="E58" t="s">
+        <v>27</v>
+      </c>
+      <c r="F58" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" t="s">
+        <v>33</v>
+      </c>
+      <c r="H58" t="s">
+        <v>12</v>
+      </c>
+      <c r="I58" t="s">
+        <v>12</v>
+      </c>
+      <c r="J58" t="s">
+        <v>12</v>
+      </c>
+      <c r="K58" t="s">
+        <v>12</v>
+      </c>
+      <c r="L58" t="s">
+        <v>12</v>
+      </c>
+      <c r="M58" t="s">
+        <v>12</v>
+      </c>
+      <c r="N58" t="s">
+        <v>58</v>
+      </c>
+      <c r="O58" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A59" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59">
+        <v>15</v>
+      </c>
+      <c r="E59" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" t="s">
+        <v>67</v>
+      </c>
+      <c r="G59" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" t="s">
+        <v>12</v>
+      </c>
+      <c r="I59" t="s">
+        <v>27</v>
+      </c>
+      <c r="J59" t="s">
+        <v>27</v>
+      </c>
+      <c r="K59" t="s">
+        <v>25</v>
+      </c>
+      <c r="L59" t="s">
+        <v>56</v>
+      </c>
+      <c r="M59" t="s">
+        <v>25</v>
+      </c>
+      <c r="N59" t="s">
+        <v>12</v>
+      </c>
+      <c r="O59" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A60" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60">
+        <v>13</v>
+      </c>
+      <c r="E60" t="s">
+        <v>25</v>
+      </c>
+      <c r="F60" t="s">
+        <v>64</v>
+      </c>
+      <c r="G60" t="s">
+        <v>12</v>
+      </c>
+      <c r="H60" t="s">
+        <v>12</v>
+      </c>
+      <c r="I60" t="s">
+        <v>25</v>
+      </c>
+      <c r="J60" t="s">
+        <v>25</v>
+      </c>
+      <c r="K60" t="s">
+        <v>25</v>
+      </c>
+      <c r="L60" t="s">
+        <v>25</v>
+      </c>
+      <c r="M60" t="s">
+        <v>12</v>
+      </c>
+      <c r="N60" t="s">
+        <v>12</v>
+      </c>
+      <c r="O60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A61" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61">
+        <v>4</v>
+      </c>
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" t="s">
+        <v>12</v>
+      </c>
+      <c r="H61" t="s">
+        <v>12</v>
+      </c>
+      <c r="I61" t="s">
+        <v>12</v>
+      </c>
+      <c r="J61" t="s">
+        <v>12</v>
+      </c>
+      <c r="K61" t="s">
+        <v>12</v>
+      </c>
+      <c r="L61" t="s">
+        <v>12</v>
+      </c>
+      <c r="M61" t="s">
+        <v>12</v>
+      </c>
+      <c r="N61" t="s">
+        <v>12</v>
+      </c>
+      <c r="O61" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62">
+        <v>6</v>
+      </c>
+      <c r="E62" t="s">
+        <v>25</v>
+      </c>
+      <c r="F62" t="s">
+        <v>62</v>
+      </c>
+      <c r="G62" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62" t="s">
+        <v>12</v>
+      </c>
+      <c r="I62" t="s">
+        <v>25</v>
+      </c>
+      <c r="J62" t="s">
+        <v>25</v>
+      </c>
+      <c r="K62" t="s">
+        <v>27</v>
+      </c>
+      <c r="L62" t="s">
+        <v>27</v>
+      </c>
+      <c r="M62" t="s">
+        <v>12</v>
+      </c>
+      <c r="N62" t="s">
+        <v>12</v>
+      </c>
+      <c r="O62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A63" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" t="s">
+        <v>38</v>
+      </c>
+      <c r="C63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>25</v>
+      </c>
+      <c r="F63" t="s">
+        <v>65</v>
+      </c>
+      <c r="G63" t="s">
+        <v>12</v>
+      </c>
+      <c r="H63" t="s">
+        <v>12</v>
+      </c>
+      <c r="I63" t="s">
+        <v>27</v>
+      </c>
+      <c r="J63" t="s">
+        <v>27</v>
+      </c>
+      <c r="K63" t="s">
+        <v>25</v>
+      </c>
+      <c r="L63" t="s">
+        <v>25</v>
+      </c>
+      <c r="M63" t="s">
+        <v>12</v>
+      </c>
+      <c r="N63" t="s">
+        <v>12</v>
+      </c>
+      <c r="O63" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A64" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64" t="s">
+        <v>39</v>
+      </c>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64">
+        <v>15</v>
+      </c>
+      <c r="E64" t="s">
+        <v>27</v>
+      </c>
+      <c r="F64" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" t="s">
+        <v>40</v>
+      </c>
+      <c r="H64" t="s">
+        <v>12</v>
+      </c>
+      <c r="I64" t="s">
+        <v>12</v>
+      </c>
+      <c r="J64" t="s">
+        <v>12</v>
+      </c>
+      <c r="K64" t="s">
+        <v>12</v>
+      </c>
+      <c r="L64" t="s">
+        <v>12</v>
+      </c>
+      <c r="M64" t="s">
+        <v>27</v>
+      </c>
+      <c r="N64" t="s">
+        <v>12</v>
+      </c>
+      <c r="O64" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A65" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65">
+        <v>12</v>
+      </c>
+      <c r="E65" t="s">
+        <v>25</v>
+      </c>
+      <c r="F65" t="s">
+        <v>77</v>
+      </c>
+      <c r="G65" t="s">
+        <v>12</v>
+      </c>
+      <c r="H65" t="s">
+        <v>12</v>
+      </c>
+      <c r="I65" t="s">
+        <v>25</v>
+      </c>
+      <c r="J65" t="s">
+        <v>25</v>
+      </c>
+      <c r="K65" t="s">
+        <v>25</v>
+      </c>
+      <c r="L65" t="s">
+        <v>27</v>
+      </c>
+      <c r="M65" t="s">
+        <v>12</v>
+      </c>
+      <c r="N65" t="s">
+        <v>12</v>
+      </c>
+      <c r="O65" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A66" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66">
+        <v>8</v>
+      </c>
+      <c r="E66" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" t="s">
+        <v>12</v>
+      </c>
+      <c r="H66" t="s">
+        <v>12</v>
+      </c>
+      <c r="I66" t="s">
+        <v>12</v>
+      </c>
+      <c r="J66" t="s">
+        <v>12</v>
+      </c>
+      <c r="K66" t="s">
+        <v>12</v>
+      </c>
+      <c r="L66" t="s">
+        <v>12</v>
+      </c>
+      <c r="M66" t="s">
+        <v>12</v>
+      </c>
+      <c r="N66" t="s">
+        <v>12</v>
+      </c>
+      <c r="O66" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" t="s">
+        <v>29</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67">
+        <v>8</v>
+      </c>
+      <c r="E67" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" t="s">
+        <v>12</v>
+      </c>
+      <c r="I67" t="s">
+        <v>12</v>
+      </c>
+      <c r="J67" t="s">
+        <v>12</v>
+      </c>
+      <c r="K67" t="s">
+        <v>12</v>
+      </c>
+      <c r="L67" t="s">
+        <v>12</v>
+      </c>
+      <c r="M67" t="s">
+        <v>12</v>
+      </c>
+      <c r="N67" t="s">
+        <v>12</v>
+      </c>
+      <c r="O67" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A68" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" t="s">
+        <v>29</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68">
+        <v>8</v>
+      </c>
+      <c r="E68" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68" t="s">
+        <v>12</v>
+      </c>
+      <c r="I68" t="s">
+        <v>12</v>
+      </c>
+      <c r="J68" t="s">
+        <v>12</v>
+      </c>
+      <c r="K68" t="s">
+        <v>12</v>
+      </c>
+      <c r="L68" t="s">
+        <v>12</v>
+      </c>
+      <c r="M68" t="s">
+        <v>12</v>
+      </c>
+      <c r="N68" t="s">
+        <v>12</v>
+      </c>
+      <c r="O68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A69" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69">
+        <v>8</v>
+      </c>
+      <c r="E69" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" t="s">
+        <v>12</v>
+      </c>
+      <c r="H69" t="s">
+        <v>12</v>
+      </c>
+      <c r="I69" t="s">
+        <v>12</v>
+      </c>
+      <c r="J69" t="s">
+        <v>12</v>
+      </c>
+      <c r="K69" t="s">
+        <v>12</v>
+      </c>
+      <c r="L69" t="s">
+        <v>12</v>
+      </c>
+      <c r="M69" t="s">
+        <v>12</v>
+      </c>
+      <c r="N69" t="s">
+        <v>12</v>
+      </c>
+      <c r="O69" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" t="s">
+        <v>29</v>
+      </c>
+      <c r="C70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70">
+        <v>8</v>
+      </c>
+      <c r="E70" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70" t="s">
+        <v>12</v>
+      </c>
+      <c r="I70" t="s">
+        <v>12</v>
+      </c>
+      <c r="J70" t="s">
+        <v>12</v>
+      </c>
+      <c r="K70" t="s">
+        <v>12</v>
+      </c>
+      <c r="L70" t="s">
+        <v>12</v>
+      </c>
+      <c r="M70" t="s">
+        <v>12</v>
+      </c>
+      <c r="N70" t="s">
+        <v>12</v>
+      </c>
+      <c r="O70" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A71" t="s">
+        <v>16</v>
+      </c>
+      <c r="B71" t="s">
+        <v>29</v>
+      </c>
+      <c r="C71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71">
+        <v>8</v>
+      </c>
+      <c r="E71" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G71" t="s">
+        <v>12</v>
+      </c>
+      <c r="H71" t="s">
+        <v>12</v>
+      </c>
+      <c r="I71" t="s">
+        <v>12</v>
+      </c>
+      <c r="J71" t="s">
+        <v>12</v>
+      </c>
+      <c r="K71" t="s">
+        <v>12</v>
+      </c>
+      <c r="L71" t="s">
+        <v>12</v>
+      </c>
+      <c r="M71" t="s">
+        <v>12</v>
+      </c>
+      <c r="N71" t="s">
+        <v>12</v>
+      </c>
+      <c r="O71" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.75">
       <c r="B83" s="1"/>
@@ -8240,8 +10760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E5E3D4-B3C4-4861-8FC5-05A8FCCE6E1C}">
   <dimension ref="A1:J54049"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -8676,8 +11196,8 @@
       <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
-        <v>12</v>
+      <c r="D14">
+        <v>6</v>
       </c>
       <c r="E14" t="s">
         <v>74</v>

</xml_diff>